<commit_message>
changing parser and adding new ones for more functionality
</commit_message>
<xml_diff>
--- a/data/Algo_6_24.xlsx
+++ b/data/Algo_6_24.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1208,7 +1208,7 @@
         <v/>
       </c>
       <c r="AB3" s="1" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AC3" s="1" t="n">
         <v>0</v>
@@ -1235,7 +1235,7 @@
         <v/>
       </c>
       <c r="AK3" s="1" t="n">
-        <v>7</v>
+        <v/>
       </c>
       <c r="AL3" s="1" t="n">
         <v/>
@@ -1437,7 +1437,7 @@
         <v/>
       </c>
       <c r="AK4" s="1" t="n">
-        <v>7</v>
+        <v/>
       </c>
       <c r="AL4" s="1" t="n">
         <v/>
@@ -1639,7 +1639,7 @@
         <v/>
       </c>
       <c r="AK5" s="1" t="n">
-        <v>1</v>
+        <v/>
       </c>
       <c r="AL5" s="1" t="n">
         <v/>
@@ -1841,7 +1841,7 @@
         <v/>
       </c>
       <c r="AK6" s="1" t="n">
-        <v>3.5</v>
+        <v/>
       </c>
       <c r="AL6" s="1" t="n">
         <v/>
@@ -2043,7 +2043,7 @@
         <v/>
       </c>
       <c r="AK7" s="1" t="n">
-        <v>3</v>
+        <v/>
       </c>
       <c r="AL7" s="1" t="n">
         <v/>

</xml_diff>